<commit_message>
Changed Business Email to use Kap's email address
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC09F8C-EAE1-474E-B43D-51EDAF1C22BF}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2B88F5F-EDFD-4626-8719-D6AC6E2A67F5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,13 +185,13 @@
     <t>Business_Email</t>
   </si>
   <si>
-    <t>noah.mangahas@accesshq.com</t>
-  </si>
-  <si>
     <t>ReportFilePath</t>
   </si>
   <si>
     <t>Data\Output\Results.xlsx</t>
+  </si>
+  <si>
+    <t>Kapeteni.polutea@accesshq.com</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -672,16 +672,16 @@
         <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>